<commit_message>
Dugnadsfelt opprettet Dato/tid kun i arrangementer
</commit_message>
<xml_diff>
--- a/Source/VariousSupporting/Navn og passord.xlsx
+++ b/Source/VariousSupporting/Navn og passord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MaineBoat\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerha\Documents\MaineBoat\Source\VariousSupporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C25514-2447-48BB-A2A4-C2931395A7FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3E642-9B42-4710-A95F-8BF1C046005F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="4980" yWindow="2565" windowWidth="22755" windowHeight="11325" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,15 +90,9 @@
     <t>Roma1995</t>
   </si>
   <si>
-    <t>105881_uw64067</t>
-  </si>
-  <si>
     <t>admintest-105881.mssql.stwcp.net</t>
   </si>
   <si>
-    <t>105881_mc66918</t>
-  </si>
-  <si>
     <t>105881_jr87416</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
     <t>105881_od92908</t>
   </si>
   <si>
-    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admintest-105881.mssql.stwcp.net;UID=105881_kr28513;PWD=Maine1953;APP=Microsoft Office;DATABASE=DB_A46E6D_Admin;</t>
-  </si>
-  <si>
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=pms-105881.mssql.stwcp.net;UID=105881-sc66800;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-pms;</t>
   </si>
   <si>
@@ -198,7 +189,16 @@
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=pvstest-105881.mssql.stwcp.net;UID=105881-eh47088;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-pvstest;</t>
   </si>
   <si>
-    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admintest-105881.mssql.stwcp.net;UID=105881-mc66918;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-admintest;</t>
+    <t>105881_av56092</t>
+  </si>
+  <si>
+    <t>105881_mj42632</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admin-105881.mssql.stwcp.net;UID=105881_kr28513;PWD=Maine1953;APP=Microsoft Office;DATABASE=10588_admin;</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admintest-105881.mssql.stwcp.net;UID=105881-mj42632;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-admintest;</t>
   </si>
 </sst>
 </file>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4541937-B5CE-4A20-80A9-B8C27113714F}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,44 +801,44 @@
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
       <c r="E2" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
       <c r="H2" s="23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="17"/>
       <c r="K2" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="19"/>
       <c r="E3" s="25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="19"/>
       <c r="H3" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="19"/>
       <c r="K3" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="19"/>
@@ -952,17 +952,17 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
       <c r="E7" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
       <c r="H7" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
@@ -970,17 +970,17 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
       <c r="E8" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>20</v>
@@ -999,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>20</v>
@@ -1008,7 +1008,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>20</v>
@@ -1022,21 +1022,21 @@
         <v>1</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>18</v>
@@ -1048,7 +1048,7 @@
       <c r="C11" s="11"/>
       <c r="D11" s="27"/>
       <c r="E11" s="23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
@@ -1061,7 +1061,7 @@
       <c r="C12" s="11"/>
       <c r="D12" s="27"/>
       <c r="E12" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
@@ -1074,7 +1074,7 @@
       <c r="C13" s="11"/>
       <c r="D13" s="27"/>
       <c r="E13" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>20</v>
@@ -1089,7 +1089,7 @@
       <c r="C14" s="11"/>
       <c r="D14" s="27"/>
       <c r="E14" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>18</v>
@@ -1106,7 +1106,7 @@
       <c r="C15" s="11"/>
       <c r="D15" s="27"/>
       <c r="E15" s="23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
@@ -1119,7 +1119,7 @@
       <c r="C16" s="11"/>
       <c r="D16" s="27"/>
       <c r="E16" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="19"/>
@@ -1132,7 +1132,7 @@
       <c r="C17" s="11"/>
       <c r="D17" s="27"/>
       <c r="E17" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>20</v>
@@ -1147,7 +1147,7 @@
       <c r="C18" s="11"/>
       <c r="D18" s="27"/>
       <c r="E18" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>18</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1182,18 +1182,18 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G25" s="2"/>
       <c r="J25" s="2"/>
@@ -1201,24 +1201,24 @@
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G26" s="2"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diverse kalenderarbeider og kontingent
</commit_message>
<xml_diff>
--- a/Source/VariousSupporting/Navn og passord.xlsx
+++ b/Source/VariousSupporting/Navn og passord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerha\Documents\MaineBoat\Source\VariousSupporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3E642-9B42-4710-A95F-8BF1C046005F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2058C54A-9299-4E8E-A7F5-891AB03F29B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="2565" windowWidth="22755" windowHeight="11325" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,10 +195,10 @@
     <t>105881_mj42632</t>
   </si>
   <si>
-    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admin-105881.mssql.stwcp.net;UID=105881_kr28513;PWD=Maine1953;APP=Microsoft Office;DATABASE=10588_admin;</t>
-  </si>
-  <si>
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admintest-105881.mssql.stwcp.net;UID=105881-mj42632;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-admintest;</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admin-105881.mssql.stwcp.net;UID=105881_kr28513;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-admin;</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,12 +1172,12 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Overgang til ny versjon VF
</commit_message>
<xml_diff>
--- a/Source/VariousSupporting/Navn og passord.xlsx
+++ b/Source/VariousSupporting/Navn og passord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerha\Documents\MaineBoat\Source\VariousSupporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2058C54A-9299-4E8E-A7F5-891AB03F29B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9181CD64-4690-416D-8AAF-7A5118F8C4E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
+    <workbookView xWindow="3240" yWindow="5295" windowWidth="26370" windowHeight="11625" xr2:uid="{B0BC954F-E872-4AD9-8DED-6C96764371E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Eier</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Win+tast</t>
   </si>
   <si>
-    <t>105881_sc66800</t>
-  </si>
-  <si>
-    <t>105881_tp18426</t>
-  </si>
-  <si>
     <t>105881_kr28513</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>105881_lr36979</t>
   </si>
   <si>
-    <t>105881_se46208</t>
-  </si>
-  <si>
     <t>105881_uq14596</t>
   </si>
   <si>
@@ -90,27 +81,6 @@
     <t>Roma1995</t>
   </si>
   <si>
-    <t>admintest-105881.mssql.stwcp.net</t>
-  </si>
-  <si>
-    <t>105881_jr87416</t>
-  </si>
-  <si>
-    <t>selskaptest-105881.mssql.stwcp.net</t>
-  </si>
-  <si>
-    <t>pmstest-105881.mssql.stwcp.net</t>
-  </si>
-  <si>
-    <t>105881_ff92174</t>
-  </si>
-  <si>
-    <t>105881_wa57856</t>
-  </si>
-  <si>
-    <t>105881_od92908</t>
-  </si>
-  <si>
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=pms-105881.mssql.stwcp.net;UID=105881-sc66800;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-pms;</t>
   </si>
   <si>
@@ -129,9 +99,6 @@
     <t>admin-105881.mssql.stwcp.net</t>
   </si>
   <si>
-    <t>pms-105881.mssql.stwcp.net</t>
-  </si>
-  <si>
     <t>selskap-105881.mssql.stwcp.net</t>
   </si>
   <si>
@@ -141,21 +108,9 @@
     <t>M314Admin</t>
   </si>
   <si>
-    <t>M314AdminTest</t>
-  </si>
-  <si>
-    <t>M314PMS</t>
-  </si>
-  <si>
-    <t>M314PMSTest</t>
-  </si>
-  <si>
     <t>M314Selskap</t>
   </si>
   <si>
-    <t>M314SelskapTest</t>
-  </si>
-  <si>
     <t>M314Sponsor</t>
   </si>
   <si>
@@ -174,31 +129,52 @@
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=pvs-105881.mssql.stwcp.net;UID=105881-ah72261;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-pvs;</t>
   </si>
   <si>
-    <t>M314PVSTest</t>
-  </si>
-  <si>
-    <t>pvstest-105881.mssql.stwcp.net</t>
-  </si>
-  <si>
-    <t>105881_fv96955</t>
-  </si>
-  <si>
-    <t>105881_eh47088</t>
-  </si>
-  <si>
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=pvstest-105881.mssql.stwcp.net;UID=105881-eh47088;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-pvstest;</t>
   </si>
   <si>
-    <t>105881_av56092</t>
-  </si>
-  <si>
-    <t>105881_mj42632</t>
-  </si>
-  <si>
-    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admintest-105881.mssql.stwcp.net;UID=105881-mj42632;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-admintest;</t>
-  </si>
-  <si>
     <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=admin-105881.mssql.stwcp.net;UID=105881_kr28513;PWD=Maine1953;APP=Microsoft Office;DATABASE=105881-admin;</t>
+  </si>
+  <si>
+    <t>Oslo2020</t>
+  </si>
+  <si>
+    <t>venner-105881.mssql.stwcp.net</t>
+  </si>
+  <si>
+    <t>105881_jn67273</t>
+  </si>
+  <si>
+    <t>105881_yb31958</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=venner-105881.mssql.stwcp.net;UID=105881_yb31958;PWD=Oslo2020;APP=Microsoft Office;DATABASE=105881-venner;</t>
+  </si>
+  <si>
+    <t>vennertest-105881.mssql.stwcp.net</t>
+  </si>
+  <si>
+    <t>105881_ox92272</t>
+  </si>
+  <si>
+    <t>105881_xy60936</t>
+  </si>
+  <si>
+    <t>M314VF</t>
+  </si>
+  <si>
+    <t>M314VFTest</t>
+  </si>
+  <si>
+    <t>M314VFParty</t>
+  </si>
+  <si>
+    <t>M314VFPartyTest</t>
+  </si>
+  <si>
+    <t>ODBC;DRIVER=SQL Server Native Client 10.0;SERVER=vennertest-105881.mssql.stwcp.net;UID=105881_xy60936;PWD=Oslo2020;APP=Microsoft Office;DATABASE=105881-vennertest;</t>
+  </si>
+  <si>
+    <t>Oslo</t>
   </si>
 </sst>
 </file>
@@ -740,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4541937-B5CE-4A20-80A9-B8C27113714F}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,44 +777,40 @@
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="23" t="s">
-        <v>39</v>
-      </c>
+      <c r="E2" s="23"/>
       <c r="F2" s="16"/>
       <c r="G2" s="17"/>
       <c r="H2" s="23" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="17"/>
       <c r="K2" s="23" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="25" t="s">
-        <v>34</v>
-      </c>
+      <c r="E3" s="25"/>
       <c r="F3" s="18"/>
       <c r="G3" s="19"/>
       <c r="H3" s="25" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="19"/>
       <c r="K3" s="25" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="19"/>
@@ -848,31 +820,27 @@
         <v>0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="E4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="12"/>
       <c r="H4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M4" s="12"/>
     </row>
@@ -881,107 +849,83 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="12">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="12">
-        <v>5</v>
-      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="12">
+        <v>8</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="12">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="L5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="12">
-        <v>3</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="22"/>
-      <c r="E6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>19</v>
-      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="22"/>
       <c r="H6" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>38</v>
-      </c>
+      <c r="B7" s="23"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="23" t="s">
-        <v>40</v>
-      </c>
+      <c r="E7" s="23"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="24" t="s">
-        <v>42</v>
-      </c>
+      <c r="H7" s="24"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
-        <v>21</v>
-      </c>
+      <c r="B8" s="26"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="25" t="s">
-        <v>24</v>
-      </c>
+      <c r="E8" s="25"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="25" t="s">
-        <v>23</v>
-      </c>
+      <c r="H8" s="25"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
@@ -989,175 +933,185 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="12">
-        <v>8</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="12">
-        <v>6</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="12">
-        <v>2</v>
-      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="27"/>
+      <c r="B11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="23" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="27"/>
+      <c r="H11" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="27"/>
+      <c r="B12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="25" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="27"/>
+      <c r="H12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="27"/>
+      <c r="B13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
       <c r="E13" s="10" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" s="12"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="27"/>
+      <c r="H13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="27"/>
+      <c r="B14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="28" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="30">
-        <v>9</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="23" t="s">
-        <v>49</v>
-      </c>
+      <c r="B15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="27"/>
+      <c r="H15" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="25" t="s">
-        <v>50</v>
-      </c>
+      <c r="B16" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="18"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="27"/>
+      <c r="H16" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="B17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="27"/>
+      <c r="H17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="30">
-        <v>4</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="27"/>
+      <c r="B18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
@@ -1172,53 +1126,64 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>56</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>28</v>
-      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="J25" s="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="G26" s="2"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
-        <v>30</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K29" t="s">
-        <v>31</v>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>